<commit_message>
Uploaded files for V1.1 and other smaller updates
</commit_message>
<xml_diff>
--- a/Hardware/Atmega32u4 - IO List.xlsx
+++ b/Hardware/Atmega32u4 - IO List.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="494" documentId="11_AD4DD024A17053AB440FF4E61151DC0A683EDF37" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{61032463-B638-4AF0-8982-EE94F60F5B68}"/>
+  <xr:revisionPtr revIDLastSave="496" documentId="11_AD4DD024A17053AB440FF4E61151DC0A683EDF37" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{DDAE5D57-84D0-4A5B-9B9C-B85DEC30A06B}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="110">
   <si>
     <t>Pinout Diffenition from MCU To Board</t>
   </si>
@@ -282,9 +282,6 @@
     <t>SPI CS</t>
   </si>
   <si>
-    <t>Open Corsair Lighting Pro / Comander Pro</t>
-  </si>
-  <si>
     <t>Fan PWM 1-6</t>
   </si>
   <si>
@@ -352,6 +349,12 @@
   </si>
   <si>
     <t>+5v USB</t>
+  </si>
+  <si>
+    <t>Open Corsair Lighting Node Pro / Comander Pro</t>
+  </si>
+  <si>
+    <t>Prefered Use:</t>
   </si>
 </sst>
 </file>
@@ -670,6 +673,8 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -697,8 +702,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1082,8 +1085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,34 +1101,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="29"/>
+      <c r="A1" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="31"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="32"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
-        <v>106</v>
-      </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
+      <c r="A3" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="F3" s="37"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -1163,7 +1168,7 @@
       <c r="F5" s="12"/>
       <c r="H5" s="8"/>
       <c r="I5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1178,12 +1183,12 @@
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1203,7 +1208,7 @@
       <c r="F7" s="14"/>
       <c r="H7" s="10"/>
       <c r="I7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1240,7 +1245,7 @@
       <c r="F9" s="9"/>
       <c r="H9" s="13"/>
       <c r="I9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1318,7 +1323,7 @@
       <c r="F13" s="12"/>
       <c r="H13" s="17"/>
       <c r="I13" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1338,7 +1343,7 @@
       <c r="F14" s="12"/>
       <c r="H14" s="18"/>
       <c r="I14" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1371,9 +1376,9 @@
         <v>84</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="F16" s="36"/>
+        <v>88</v>
+      </c>
+      <c r="F16" s="27"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
@@ -1469,7 +1474,7 @@
         <v>67</v>
       </c>
       <c r="E22" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F22" s="8"/>
     </row>
@@ -1500,7 +1505,7 @@
         <v>69</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E24" s="23"/>
       <c r="F24" s="12"/>
@@ -1516,7 +1521,7 @@
         <v>70</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E25" s="23"/>
       <c r="F25" s="12"/>
@@ -1581,7 +1586,7 @@
       </c>
       <c r="D29" s="22"/>
       <c r="E29" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F29" s="13"/>
     </row>
@@ -1597,7 +1602,7 @@
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F30" s="13"/>
     </row>
@@ -1613,9 +1618,9 @@
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="F31" s="36"/>
+        <v>89</v>
+      </c>
+      <c r="F31" s="27"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
@@ -1643,7 +1648,7 @@
       </c>
       <c r="D33" s="22"/>
       <c r="E33" s="23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F33" s="8"/>
     </row>
@@ -1659,7 +1664,7 @@
       </c>
       <c r="D34" s="22"/>
       <c r="E34" s="23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F34" s="8"/>
     </row>
@@ -1675,9 +1680,9 @@
       </c>
       <c r="D35" s="22"/>
       <c r="E35" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="F35" s="37"/>
+        <v>92</v>
+      </c>
+      <c r="F35" s="28"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
@@ -1691,7 +1696,7 @@
       </c>
       <c r="D36" s="22"/>
       <c r="E36" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F36" s="8"/>
     </row>
@@ -1755,7 +1760,7 @@
       </c>
       <c r="D40" s="22"/>
       <c r="E40" s="23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F40" s="10"/>
     </row>
@@ -1771,7 +1776,7 @@
       </c>
       <c r="D41" s="22"/>
       <c r="E41" s="23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F41" s="10"/>
     </row>
@@ -1787,7 +1792,7 @@
       </c>
       <c r="D42" s="22"/>
       <c r="E42" s="23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F42" s="10"/>
     </row>
@@ -1803,7 +1808,7 @@
       </c>
       <c r="D43" s="22"/>
       <c r="E43" s="23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F43" s="10"/>
     </row>

</xml_diff>